<commit_message>
commonName auth  A1#070103000000XX subject_application_vendor ASL3 Genovese subject_application_id SivisWeb subject_application_version v.2.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#070103000000XX/ASL3_Genovese/SivisWeb/v.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#070103000000XX/ASL3_Genovese/SivisWeb/v.2.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabat\Desktop\it-fse-accreditamento\GATEWAY\A1#070103000000XX\ASL3_Genovese\SivisWeb\v.2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B9FA48-E324-4DFA-B490-F1756E6E40CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A044D76A-A043-4D89-9A03-392F363ABDE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7788" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,78 +803,6 @@
     <t>Il software non gestisce la sezione opzionale “Quesito Diagnostico”</t>
   </si>
   <si>
-    <t>291cd9ddb3b2ee4e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.af36d8a26a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>684553294f015386</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.643d29f91f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>085c5a4985b130d3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.b9b9d3bbf4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e43302528fc422da</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.16d6a98430^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>103e48f0f59af7f0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.584ec098fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>d00c513943b9902a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ba0cfa58b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>c5d0604afdc3cce8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.68f037df4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>86a1f81cedf3c0ee</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.c0ac140fb4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f5b81349274c4b12</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.f502fdffe7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>a629022361597978</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9bf04f4b32^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>52996f76fa4722ce</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.a8e073dcf2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>491b2108e9b2facc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.7b9977894e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>DATO OBBLIGATORIO MANCANTE O ERRATO!</t>
   </si>
   <si>
@@ -892,58 +820,130 @@
     <t>Il flusso produttivo del referto non viene interrotto. Il referto viene contrassegnato come non validato per FSE e processato successivamente ai fini della validazione.</t>
   </si>
   <si>
-    <t>2024-05-14T12:02:46Z</t>
-  </si>
-  <si>
-    <t>e43b331b56b5dece</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2024-05-14T12:04:01Z</t>
-  </si>
-  <si>
-    <t>feabadfad0bedd81</t>
-  </si>
-  <si>
     <t>2024-05-14T12:05:00Z</t>
   </si>
   <si>
-    <t>2024-05-13T17:42:30Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:45:14Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:47:55</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:49:16Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:51:06Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:54:54Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:56:32Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:58:34Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T18:00:43Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T18:02:21Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T18:03:31Z</t>
-  </si>
-  <si>
-    <t>2024-05-13T17:41:34Z</t>
+    <t>2024-05-16T11:56:09Z</t>
+  </si>
+  <si>
+    <t>399c146bd4e504f6</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:59:14Z</t>
+  </si>
+  <si>
+    <t>2f419df12677a0ee</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:01:47Z</t>
+  </si>
+  <si>
+    <t>cbcec424ca11f948</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9b706d82e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:09:13Z</t>
+  </si>
+  <si>
+    <t>df94948122b40be9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.bdc4c8efd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:13:13Z</t>
+  </si>
+  <si>
+    <t>cec12822cd345a52</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.b777c31bb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:21:45Z</t>
+  </si>
+  <si>
+    <t>6db32be01c103737</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1cf1ce5ca5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:23:29Z</t>
+  </si>
+  <si>
+    <t>9b6570f464fcbb7d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.7940ba4988^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:24:59Z</t>
+  </si>
+  <si>
+    <t>a1ba3e46c02e629c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.6a987fc921^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:27:57Z</t>
+  </si>
+  <si>
+    <t>8714a2932fa575dd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.b678c3f96f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:37:51Z</t>
+  </si>
+  <si>
+    <t>676da5e6e84d2838</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.f95b06e744^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:41:57Z</t>
+  </si>
+  <si>
+    <t>57bd8f0023d8e449</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.a134476b47^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:47:56Z</t>
+  </si>
+  <si>
+    <t>d8d721b96fa5e1d5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.57e860cf13^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T11:50:19Z</t>
+  </si>
+  <si>
+    <t>73cbf32ee246afee</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.66467a9fc3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T10:58:09Z</t>
+  </si>
+  <si>
+    <t>8ca449f4af565233</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.affe9fa64b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1393,6 +1393,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1415,7 +1418,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -3898,10 +3901,10 @@
   <dimension ref="A1:T653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomRight" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3939,12 +3942,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3962,14 +3965,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3987,12 +3990,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="48" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4011,12 +4014,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4034,8 +4037,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4169,16 +4172,16 @@
         <v>56</v>
       </c>
       <c r="F10" s="23">
-        <v>45426</v>
-      </c>
-      <c r="G10" s="49" t="s">
-        <v>201</v>
+        <v>45428</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>179</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="J10" s="35" t="s">
         <v>60</v>
@@ -4195,7 +4198,7 @@
         <v>60</v>
       </c>
       <c r="P10" s="35" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="26"/>
@@ -4221,16 +4224,16 @@
         <v>58</v>
       </c>
       <c r="F11" s="23">
-        <v>45426</v>
-      </c>
-      <c r="G11" s="49" t="s">
-        <v>204</v>
+        <v>45428</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>181</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="J11" s="35" t="s">
         <v>60</v>
@@ -4247,7 +4250,7 @@
         <v>60</v>
       </c>
       <c r="P11" s="35" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="26"/>
@@ -4275,8 +4278,8 @@
       <c r="F12" s="23">
         <v>45426</v>
       </c>
-      <c r="G12" s="49" t="s">
-        <v>206</v>
+      <c r="G12" s="37" t="s">
+        <v>178</v>
       </c>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
@@ -4295,7 +4298,7 @@
         <v>60</v>
       </c>
       <c r="P12" s="35" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="26" t="s">
@@ -4323,16 +4326,16 @@
         <v>63</v>
       </c>
       <c r="F13" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>60</v>
@@ -4481,16 +4484,16 @@
         <v>71</v>
       </c>
       <c r="F17" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>60</v>
@@ -4507,7 +4510,7 @@
         <v>60</v>
       </c>
       <c r="P17" s="35" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4533,16 +4536,16 @@
         <v>73</v>
       </c>
       <c r="F18" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>60</v>
@@ -4555,13 +4558,13 @@
         <v>60</v>
       </c>
       <c r="N18" s="36" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="O18" s="35" t="s">
         <v>163</v>
       </c>
       <c r="P18" s="35" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -4587,16 +4590,16 @@
         <v>75</v>
       </c>
       <c r="F19" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>60</v>
@@ -4613,7 +4616,7 @@
         <v>60</v>
       </c>
       <c r="P19" s="35" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -4639,16 +4642,16 @@
         <v>77</v>
       </c>
       <c r="F20" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>60</v>
@@ -4661,13 +4664,13 @@
         <v>60</v>
       </c>
       <c r="N20" s="36" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="O20" s="35" t="s">
         <v>163</v>
       </c>
       <c r="P20" s="35" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4693,16 +4696,16 @@
         <v>79</v>
       </c>
       <c r="F21" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>60</v>
@@ -4715,13 +4718,13 @@
         <v>60</v>
       </c>
       <c r="N21" s="36" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="O21" s="35" t="s">
         <v>163</v>
       </c>
       <c r="P21" s="35" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -4747,16 +4750,16 @@
         <v>81</v>
       </c>
       <c r="F22" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>60</v>
@@ -4769,13 +4772,13 @@
         <v>60</v>
       </c>
       <c r="N22" s="36" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="O22" s="35" t="s">
         <v>163</v>
       </c>
       <c r="P22" s="35" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
@@ -4915,16 +4918,16 @@
         <v>89</v>
       </c>
       <c r="F26" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>60</v>
@@ -4937,13 +4940,13 @@
         <v>60</v>
       </c>
       <c r="N26" s="36" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="O26" s="35" t="s">
         <v>163</v>
       </c>
       <c r="P26" s="35" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
@@ -4969,16 +4972,16 @@
         <v>91</v>
       </c>
       <c r="F27" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>60</v>
@@ -4991,13 +4994,13 @@
         <v>60</v>
       </c>
       <c r="N27" s="36" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="O27" s="35" t="s">
         <v>163</v>
       </c>
       <c r="P27" s="35" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -5061,16 +5064,16 @@
         <v>95</v>
       </c>
       <c r="F29" s="23">
-        <v>45425</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>216</v>
+        <v>45428</v>
+      </c>
+      <c r="G29" s="37" t="s">
+        <v>210</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>60</v>
@@ -5083,13 +5086,13 @@
         <v>60</v>
       </c>
       <c r="N29" s="36" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="O29" s="35" t="s">
         <v>163</v>
       </c>
       <c r="P29" s="35" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="26"/>
@@ -5305,16 +5308,16 @@
         <v>107</v>
       </c>
       <c r="F35" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>217</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>194</v>
+        <v>213</v>
+      </c>
+      <c r="H35" s="50" t="s">
+        <v>214</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="J35" s="25" t="s">
         <v>60</v>
@@ -5331,7 +5334,7 @@
         <v>60</v>
       </c>
       <c r="P35" s="35" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -5357,16 +5360,16 @@
         <v>109</v>
       </c>
       <c r="F36" s="23">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="G36" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="I36" s="24" t="s">
         <v>218</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>173</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>60</v>

</xml_diff>